<commit_message>
Changes as per those requested by Humus specialist BLW.
</commit_message>
<xml_diff>
--- a/src/eCH_0267__1_0__Rechner.xlsx
+++ b/src/eCH_0267__1_0__Rechner.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\depot\isceco\blw\dnpsm\dnpsm-ech\dnpsm-ech-docs\docs\rechner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\depot\isceco\blw-ofag-ufag\eCH-0267\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C622F43-3F02-4CA3-88E5-9FCE315B5FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA8B479-AB12-497D-BDF7-43E52F149E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38890" yWindow="2300" windowWidth="32330" windowHeight="21370" tabRatio="849" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29220" yWindow="2175" windowWidth="26985" windowHeight="15353" tabRatio="849" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mainNutrient" sheetId="22" r:id="rId1"/>
     <sheet name="nutrientAreaRequirementType" sheetId="33" r:id="rId2"/>
     <sheet name="embeddedAmmonia" sheetId="3" r:id="rId3"/>
     <sheet name="mainHumus" sheetId="18" r:id="rId4"/>
-    <sheet name="fertiliserDilution" sheetId="30" r:id="rId5"/>
+    <sheet name="manureDilution" sheetId="30" r:id="rId5"/>
     <sheet name="calcParameterTypeAmmonia" sheetId="17" r:id="rId6"/>
     <sheet name="calcParameterCategoryAmmonia" sheetId="16" r:id="rId7"/>
     <sheet name="calcParameterTypeNutrient" sheetId="31" r:id="rId8"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="670">
   <si>
     <t>Beispiel</t>
   </si>
@@ -1357,15 +1357,6 @@
     <t>catchCrop</t>
   </si>
   <si>
-    <t>eCH:0263:manureRecyclingProducttype:id</t>
-  </si>
-  <si>
-    <t>appliedQuantity_inKg</t>
-  </si>
-  <si>
-    <t>mengeAngewendet_inKg</t>
-  </si>
-  <si>
     <t>DüngerHumus</t>
   </si>
   <si>
@@ -1522,9 +1513,6 @@
     <t>A list of humus calculations per area/directPaymentCrop. These flow into the related total calculation.</t>
   </si>
   <si>
-    <t>The calculation of humus accumulation.</t>
-  </si>
-  <si>
     <t>Ein Indikator</t>
   </si>
   <si>
@@ -1537,9 +1525,6 @@
     <t>A list of applied fertiliser per area.</t>
   </si>
   <si>
-    <t>The total accumulation of humus for all indicated areas of the localUnit. Negative amounts indicate a reduction in humus.</t>
-  </si>
-  <si>
     <t>The timestamp of the calculation.</t>
   </si>
   <si>
@@ -1579,27 +1564,18 @@
     <t>Indicates if the crop residues are retained on the area.</t>
   </si>
   <si>
-    <t>The humus accumulation in the unit indicated by the attribute name.</t>
-  </si>
-  <si>
     <t>catchCropCalculation</t>
   </si>
   <si>
     <t>ZwischenKulturBerechnung</t>
   </si>
   <si>
-    <t>The calculation of accumulated humus for the indicated catchCrop (specified in the parent element).</t>
-  </si>
-  <si>
     <t>The catchCrop.</t>
   </si>
   <si>
     <t>Die Zwischenkultur.</t>
   </si>
   <si>
-    <t>The humus accumulation in the unit indicated by the attribute name, reduced to a square metre.</t>
-  </si>
-  <si>
     <t>Indicates if the catchCrop was harvested or not.</t>
   </si>
   <si>
@@ -1609,45 +1585,15 @@
     <t>geerntet</t>
   </si>
   <si>
-    <t>Die zusammengefasste angewendete Düngung pro Fläche</t>
-  </si>
-  <si>
-    <t>A list of applied fertiliser for this area.</t>
-  </si>
-  <si>
-    <t>Eine Liste angewendeter Dünger für diese Fläche.</t>
-  </si>
-  <si>
     <t>appliedFertiliser</t>
   </si>
   <si>
-    <t>AngewendeteDünger</t>
-  </si>
-  <si>
-    <t>The quantity of applied fertiliser in the unit indicated in the attribute name.</t>
-  </si>
-  <si>
-    <t>Die Menge der angewendeten Düngers in der Einheit, die im Attributennamen angegeben wird.</t>
-  </si>
-  <si>
-    <t>fertiliserDilution</t>
-  </si>
-  <si>
     <t>Eine Enumeration zulässiger Verdünnungswerte angwendeter Produkttypen.</t>
   </si>
   <si>
     <t>An enumerated list of allowable dilutions of productTypes.</t>
   </si>
   <si>
-    <t>The dilution of the applied fertiliser (which is assoicated with a manureRecyclingProducttype). This will be not-NA for all productTypes that are  liquid in nature, e.g. Slurry.</t>
-  </si>
-  <si>
-    <t>Die Verdünnung des abgewendeten Düngers. Dies wird nicht-NA sein für alle Produkttypen, die flüssig sind (z.B. Gülle).</t>
-  </si>
-  <si>
-    <t>The applied fertiliser for the area indicatedin the parent element.</t>
-  </si>
-  <si>
     <t>A multi-lingual descritor of the item.</t>
   </si>
   <si>
@@ -1670,12 +1616,6 @@
   </si>
   <si>
     <t>appliedFertilisation</t>
-  </si>
-  <si>
-    <t>AngewendeteDüngung</t>
-  </si>
-  <si>
-    <t>The aggregate applied fertilisation pro area.</t>
   </si>
   <si>
     <t>DüngerVerdünnung</t>
@@ -2108,13 +2048,6 @@
     <t>productType</t>
   </si>
   <si>
-    <t>Der Produkttyp des angewendeten Hof-Rec Düngerprodukts welcher auf die Fläche angewendet wurde die im übergeordneten Element "angewendete Düngung" angegeben wird.</t>
-  </si>
-  <si>
-    <t>Frage: nur Hof-Rec?
-Die abschliessende Liste für Düngertyp ist: Kompost, Gärgut, Festes Gärgut, Flüssiges Gärgut, Mist, Mist separiert, Gülle, Gülle separiert, Gemüserüstabfälle, Ernterückstände von Gemüsekulturen, Hofdünger vergoren, Mist vergoren und separiert, Gülle vergoren und separiert</t>
-  </si>
-  <si>
     <t>Eine mehrsprachige Beschreibung</t>
   </si>
   <si>
@@ -2168,6 +2101,82 @@
   </si>
   <si>
     <t>Angabe, ob die Zwischenkultur auf der Fläche geerntet wurden oder nicht.</t>
+  </si>
+  <si>
+    <t>Die zusammengefasste ausgebrachte Düngung pro Fläche</t>
+  </si>
+  <si>
+    <t>spreadManure</t>
+  </si>
+  <si>
+    <t>spreadQuantity_inKg</t>
+  </si>
+  <si>
+    <t>manureDilution</t>
+  </si>
+  <si>
+    <t>The the change in bumus for the unit indicated by the attribute name, reduced to a square metre.</t>
+  </si>
+  <si>
+    <t>The manure spread for the area indicatedin the parent element.</t>
+  </si>
+  <si>
+    <t>The aggregate fertilisation spread pro area.</t>
+  </si>
+  <si>
+    <t>A list of manure spread for this area.</t>
+  </si>
+  <si>
+    <t>The quantity of manure spread per unit indicated in the attribute name.</t>
+  </si>
+  <si>
+    <t>The dilution of the spread manure (which is associated with a manureRecyclingProducttype). This will be not-NA for all productTypes that are  liquid in nature, e.g. Slurry.</t>
+  </si>
+  <si>
+    <t>The calculation of the change in humus content for a localUnit and its areas as per humusbilanz.ch.</t>
+  </si>
+  <si>
+    <t>The total change in humus content for all indicated areas of the localUnit. Negative amounts indicate a reduction in humus, positive amounts indicate an accumulation.</t>
+  </si>
+  <si>
+    <t>The change in humus content for the unit indicated by the attribute name.</t>
+  </si>
+  <si>
+    <t>The change in humus content for the unit indicated by the attribute name, reduced to a square metre.</t>
+  </si>
+  <si>
+    <t>The calculation of the change in humus content for the indicated catchCrop (specified in the parent element).</t>
+  </si>
+  <si>
+    <t>The naming in English is a little tricky. "Manure" was already taken by the following element, and fertilisation is any event an accurate translation of Düngung.</t>
+  </si>
+  <si>
+    <t>AusgebrachteDüngung</t>
+  </si>
+  <si>
+    <t>Eine Liste ausgebrachter Dünger für diese Fläche.</t>
+  </si>
+  <si>
+    <t>Der Produkttyp des ausgebrachten Hof-Rec Düngerprodukts welcher auf die Fläche ausgebracht wurde, die im übergeordneten Element "ausgebrachteDüngung" angegeben wird.</t>
+  </si>
+  <si>
+    <t>mengeAusgebracht_inKg</t>
+  </si>
+  <si>
+    <t>Die Menge des ausgebrachten Düngers in der Einheit, die im Attributennamen angegeben wird.</t>
+  </si>
+  <si>
+    <t>AusgebrachteDünger</t>
+  </si>
+  <si>
+    <t>Die Verdünnung des ausgebrachten Düngers. Dies wird nicht-NA sein für alle Produkttypen, die flüssig sind (z.B. Gülle).</t>
+  </si>
+  <si>
+    <t>eCH:0263:manureRecyclingProducttype:id
+with Restriction: Die abschliessende Liste für Düngertyp ist: Kompost, Gärgut, Festes Gärgut, Flüssiges Gärgut, Mist, Mist separiert, Gülle, Gülle separiert, Gemüserüstabfälle, Ernterückstände von Gemüsekulturen, Hofdünger vergoren, Mist vergoren und separiert, Gülle vergoren und separiert</t>
+  </si>
+  <si>
+    <t>Is manure a good word choice given that we may be spreading recycling product as well?</t>
   </si>
 </sst>
 </file>
@@ -3510,7 +3519,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1" ht="61.15" thickBot="1" x14ac:dyDescent="0.45">
@@ -3558,7 +3567,7 @@
       </c>
       <c r="B3" s="88"/>
       <c r="C3" s="23" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="D3" s="88"/>
       <c r="E3" s="89"/>
@@ -3566,13 +3575,13 @@
       <c r="G3" s="57"/>
       <c r="H3" s="57"/>
       <c r="I3" s="19" t="s">
-        <v>511</v>
+        <v>491</v>
       </c>
       <c r="J3" s="86" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>512</v>
+        <v>492</v>
       </c>
       <c r="L3" s="16"/>
       <c r="M3" s="16"/>
@@ -3597,11 +3606,11 @@
         <v>27</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="23" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="L4" s="17"/>
       <c r="M4"/>
@@ -3628,11 +3637,11 @@
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="23" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="23" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
@@ -3643,7 +3652,7 @@
         <v>128</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>658</v>
+        <v>636</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
@@ -3655,15 +3664,15 @@
         <v>5</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>508</v>
+        <v>488</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="23" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="23" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="L6" s="24"/>
       <c r="M6" s="2"/>
@@ -3688,11 +3697,11 @@
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="23" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="23" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="L7" s="33"/>
       <c r="M7"/>
@@ -3703,7 +3712,7 @@
         <v>346</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>534</v>
+        <v>514</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
@@ -3746,7 +3755,7 @@
       </c>
       <c r="H9" s="31"/>
       <c r="I9" s="23" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="23" t="s">
@@ -3761,7 +3770,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>532</v>
+        <v>512</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>3</v>
@@ -3769,7 +3778,7 @@
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
       <c r="G10" s="2" t="s">
-        <v>520</v>
+        <v>500</v>
       </c>
       <c r="H10" s="31"/>
       <c r="I10" s="33" t="s">
@@ -3777,17 +3786,17 @@
       </c>
       <c r="J10" s="31"/>
       <c r="K10" s="31" t="s">
-        <v>533</v>
+        <v>513</v>
       </c>
       <c r="M10" s="33"/>
     </row>
     <row r="11" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A11" s="31"/>
       <c r="B11" s="5" t="s">
-        <v>545</v>
+        <v>525</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
@@ -3808,10 +3817,10 @@
     <row r="12" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A12" s="31"/>
       <c r="B12" s="5" t="s">
-        <v>546</v>
+        <v>526</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>547</v>
+        <v>527</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>3</v>
@@ -3828,10 +3837,10 @@
     <row r="13" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A13" s="31"/>
       <c r="B13" s="5" t="s">
-        <v>556</v>
+        <v>536</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>561</v>
+        <v>541</v>
       </c>
       <c r="D13" s="32">
         <v>1</v>
@@ -3855,10 +3864,10 @@
     <row r="14" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A14" s="31"/>
       <c r="B14" s="5" t="s">
-        <v>555</v>
+        <v>535</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>562</v>
+        <v>542</v>
       </c>
       <c r="D14" s="32">
         <v>1</v>
@@ -3882,10 +3891,10 @@
     <row r="15" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A15" s="31"/>
       <c r="B15" s="5" t="s">
-        <v>554</v>
+        <v>534</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>563</v>
+        <v>543</v>
       </c>
       <c r="D15" s="32">
         <v>1</v>
@@ -3902,10 +3911,10 @@
     <row r="16" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A16" s="31"/>
       <c r="B16" s="5" t="s">
-        <v>553</v>
+        <v>533</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>564</v>
+        <v>544</v>
       </c>
       <c r="D16" s="32">
         <v>1</v>
@@ -3922,10 +3931,10 @@
     <row r="17" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A17" s="31"/>
       <c r="B17" s="5" t="s">
-        <v>552</v>
+        <v>532</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
       <c r="D17" s="32">
         <v>1</v>
@@ -3949,10 +3958,10 @@
     <row r="18" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A18" s="31"/>
       <c r="B18" s="5" t="s">
-        <v>551</v>
+        <v>531</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>566</v>
+        <v>546</v>
       </c>
       <c r="D18" s="32">
         <v>1</v>
@@ -3976,10 +3985,10 @@
     <row r="19" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A19" s="31"/>
       <c r="B19" s="5" t="s">
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>567</v>
+        <v>547</v>
       </c>
       <c r="D19" s="32">
         <v>1</v>
@@ -3996,10 +4005,10 @@
     <row r="20" spans="1:13" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A20" s="31"/>
       <c r="B20" s="5" t="s">
-        <v>549</v>
+        <v>529</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>568</v>
+        <v>548</v>
       </c>
       <c r="D20" s="32">
         <v>1</v>
@@ -4031,15 +4040,15 @@
         <v>5</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="H21" s="23"/>
       <c r="I21" s="23" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="J21" s="23"/>
       <c r="K21" s="23" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -4047,7 +4056,7 @@
     <row r="22" spans="1:13" ht="27" x14ac:dyDescent="0.35">
       <c r="A22" s="31"/>
       <c r="C22" s="5" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
@@ -4082,15 +4091,15 @@
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
       <c r="G23" s="2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H23" s="31"/>
       <c r="I23" s="23" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="J23" s="23"/>
       <c r="K23" s="23" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="L23" s="33" t="s">
         <v>34</v>
@@ -4114,11 +4123,11 @@
     </row>
     <row r="25" spans="1:13" ht="83.25" x14ac:dyDescent="0.4">
       <c r="A25" s="66" t="s">
-        <v>544</v>
+        <v>524</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="20" t="s">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
@@ -4129,7 +4138,7 @@
       <c r="J25" s="20"/>
       <c r="K25" s="20"/>
       <c r="L25" s="36" t="s">
-        <v>661</v>
+        <v>639</v>
       </c>
       <c r="M25" s="76"/>
     </row>
@@ -4151,15 +4160,15 @@
         <v>5</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H26" s="23"/>
       <c r="I26" s="17" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="J26" s="17"/>
       <c r="K26" s="17" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
@@ -4168,7 +4177,7 @@
       <c r="A27" s="25"/>
       <c r="B27" s="5"/>
       <c r="C27" s="23" t="s">
-        <v>541</v>
+        <v>521</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -4187,7 +4196,7 @@
       <c r="J27" s="17"/>
       <c r="K27" s="17"/>
       <c r="L27" s="17" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
       <c r="M27" s="17"/>
     </row>
@@ -4195,7 +4204,7 @@
       <c r="A28" s="25"/>
       <c r="B28" s="5"/>
       <c r="C28" s="23" t="s">
-        <v>542</v>
+        <v>522</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
@@ -4214,7 +4223,7 @@
       <c r="J28" s="17"/>
       <c r="K28" s="17"/>
       <c r="L28" s="12" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
       <c r="M28" s="17"/>
     </row>
@@ -4235,11 +4244,11 @@
     </row>
     <row r="30" spans="1:13" ht="83.25" x14ac:dyDescent="0.4">
       <c r="A30" s="66" t="s">
-        <v>548</v>
+        <v>528</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="20" t="s">
-        <v>547</v>
+        <v>527</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
@@ -4250,7 +4259,7 @@
       <c r="J30" s="20"/>
       <c r="K30" s="20"/>
       <c r="L30" s="36" t="s">
-        <v>661</v>
+        <v>639</v>
       </c>
       <c r="M30" s="76"/>
     </row>
@@ -4272,15 +4281,15 @@
         <v>5</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H31" s="23"/>
       <c r="I31" s="17" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="17" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="L31" s="17"/>
       <c r="M31" s="17"/>
@@ -4289,7 +4298,7 @@
       <c r="A32" s="25"/>
       <c r="B32" s="5"/>
       <c r="C32" s="23" t="s">
-        <v>541</v>
+        <v>521</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
@@ -4308,7 +4317,7 @@
       <c r="J32" s="17"/>
       <c r="K32" s="17"/>
       <c r="L32" s="17" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
       <c r="M32" s="17"/>
     </row>
@@ -4316,7 +4325,7 @@
       <c r="A33" s="25"/>
       <c r="B33" s="5"/>
       <c r="C33" s="23" t="s">
-        <v>542</v>
+        <v>522</v>
       </c>
       <c r="D33" s="5">
         <v>1</v>
@@ -4335,17 +4344,17 @@
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
       <c r="L33" s="12" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
       <c r="M33" s="17"/>
     </row>
     <row r="34" spans="1:13" s="13" customFormat="1" ht="27" x14ac:dyDescent="0.35">
       <c r="A34" s="25"/>
       <c r="B34" s="5" t="s">
-        <v>590</v>
+        <v>570</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>592</v>
+        <v>572</v>
       </c>
       <c r="D34" s="5">
         <v>1</v>
@@ -4357,13 +4366,13 @@
         <v>5</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>592</v>
+        <v>572</v>
       </c>
       <c r="H34" s="31"/>
       <c r="I34" s="31"/>
       <c r="J34" s="31"/>
       <c r="K34" s="31" t="s">
-        <v>591</v>
+        <v>571</v>
       </c>
       <c r="L34" s="17"/>
       <c r="M34" s="17"/>
@@ -4391,7 +4400,7 @@
         <v>125</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>520</v>
+        <v>500</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
@@ -4401,7 +4410,7 @@
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
       <c r="K36" s="19" t="s">
-        <v>529</v>
+        <v>509</v>
       </c>
       <c r="L36" s="19"/>
       <c r="M36" s="15"/>
@@ -4409,10 +4418,10 @@
     <row r="37" spans="1:13" s="13" customFormat="1" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A37" s="14"/>
       <c r="B37" s="38" t="s">
-        <v>531</v>
+        <v>511</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>521</v>
+        <v>501</v>
       </c>
       <c r="D37" s="5">
         <v>1</v>
@@ -4424,13 +4433,13 @@
         <v>5</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>516</v>
+        <v>496</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5" t="s">
-        <v>557</v>
+        <v>537</v>
       </c>
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
@@ -4459,10 +4468,10 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5" t="s">
-        <v>530</v>
+        <v>510</v>
       </c>
       <c r="L38" s="13" t="s">
-        <v>522</v>
+        <v>502</v>
       </c>
       <c r="M38" s="15"/>
     </row>
@@ -4537,7 +4546,7 @@
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="5" t="s">
-        <v>516</v>
+        <v>496</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
@@ -4547,7 +4556,7 @@
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
       <c r="K44" s="10" t="s">
-        <v>558</v>
+        <v>538</v>
       </c>
       <c r="L44" s="31"/>
       <c r="M44" s="31"/>
@@ -4613,10 +4622,10 @@
     <row r="47" spans="1:13" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="5" t="s">
-        <v>538</v>
+        <v>518</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>523</v>
+        <v>503</v>
       </c>
       <c r="D47" s="5">
         <v>1</v>
@@ -4628,7 +4637,7 @@
         <v>5</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>523</v>
+        <v>503</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -4641,7 +4650,7 @@
       <c r="A48" s="3"/>
       <c r="B48" s="5"/>
       <c r="C48" s="2" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="D48" s="5">
         <v>1</v>
@@ -4653,7 +4662,7 @@
         <v>5</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -4670,7 +4679,7 @@
         <v>89</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>536</v>
+        <v>516</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -4684,10 +4693,10 @@
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2" t="s">
-        <v>559</v>
+        <v>539</v>
       </c>
       <c r="L49" s="85" t="s">
-        <v>528</v>
+        <v>508</v>
       </c>
       <c r="M49" s="33"/>
     </row>
@@ -4697,7 +4706,7 @@
         <v>88</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>537</v>
+        <v>517</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>3</v>
@@ -4709,13 +4718,13 @@
         <v>5</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>569</v>
+        <v>549</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2" t="s">
-        <v>560</v>
+        <v>540</v>
       </c>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
@@ -4752,11 +4761,11 @@
     </row>
     <row r="53" spans="1:13" s="4" customFormat="1" ht="40.5" x14ac:dyDescent="0.4">
       <c r="A53" s="66" t="s">
-        <v>576</v>
+        <v>556</v>
       </c>
       <c r="B53" s="19"/>
       <c r="C53" s="20" t="s">
-        <v>523</v>
+        <v>503</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="19"/>
@@ -4766,7 +4775,7 @@
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
       <c r="K53" s="20" t="s">
-        <v>524</v>
+        <v>504</v>
       </c>
       <c r="L53" s="36"/>
       <c r="M53" s="15"/>
@@ -4774,7 +4783,7 @@
     <row r="54" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="5" t="s">
-        <v>539</v>
+        <v>519</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>139</v>
@@ -4795,7 +4804,7 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2" t="s">
-        <v>601</v>
+        <v>581</v>
       </c>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -4840,14 +4849,14 @@
       <c r="J57" s="20"/>
       <c r="K57" s="20"/>
       <c r="L57" s="36" t="s">
-        <v>540</v>
+        <v>520</v>
       </c>
       <c r="M57" s="15"/>
     </row>
     <row r="58" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="5" t="s">
-        <v>539</v>
+        <v>519</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>139</v>
@@ -4862,7 +4871,7 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2" t="s">
-        <v>601</v>
+        <v>581</v>
       </c>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
@@ -4899,11 +4908,11 @@
     </row>
     <row r="61" spans="1:13" s="4" customFormat="1" ht="54" x14ac:dyDescent="0.4">
       <c r="A61" s="66" t="s">
-        <v>593</v>
+        <v>573</v>
       </c>
       <c r="B61" s="19"/>
       <c r="C61" s="20" t="s">
-        <v>592</v>
+        <v>572</v>
       </c>
       <c r="D61" s="19"/>
       <c r="E61" s="19"/>
@@ -4913,17 +4922,17 @@
       <c r="I61" s="20"/>
       <c r="J61" s="20"/>
       <c r="K61" s="20" t="s">
-        <v>594</v>
+        <v>574</v>
       </c>
       <c r="L61" s="36" t="s">
-        <v>540</v>
+        <v>520</v>
       </c>
       <c r="M61" s="15"/>
     </row>
     <row r="62" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3"/>
       <c r="B62" s="5" t="s">
-        <v>539</v>
+        <v>519</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>139</v>
@@ -4938,7 +4947,7 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2" t="s">
-        <v>601</v>
+        <v>581</v>
       </c>
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
@@ -5009,7 +5018,7 @@
       </c>
       <c r="B67" s="19"/>
       <c r="C67" s="20" t="s">
-        <v>525</v>
+        <v>505</v>
       </c>
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
@@ -5019,7 +5028,7 @@
       <c r="I67" s="20"/>
       <c r="J67" s="20"/>
       <c r="K67" s="20" t="s">
-        <v>527</v>
+        <v>507</v>
       </c>
       <c r="L67" s="36"/>
       <c r="M67" s="15"/>
@@ -5041,7 +5050,7 @@
         <v>86</v>
       </c>
       <c r="H68" s="17" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>298</v>
@@ -5073,13 +5082,13 @@
         <v>300</v>
       </c>
       <c r="H69" s="17" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I69" s="17" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="L69" s="15"/>
       <c r="M69" s="15"/>
@@ -5107,7 +5116,7 @@
         <v>350</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>501</v>
+        <v>483</v>
       </c>
       <c r="K70" s="5" t="s">
         <v>303</v>
@@ -5139,7 +5148,7 @@
         <v>351</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="K71" s="5" t="s">
         <v>304</v>
@@ -17076,16 +17085,16 @@
         <v>371</v>
       </c>
       <c r="B2" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E2" t="s">
-        <v>575</v>
+        <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -17093,10 +17102,10 @@
         <v>372</v>
       </c>
       <c r="B3" t="s">
-        <v>571</v>
+        <v>551</v>
       </c>
       <c r="E3" t="s">
-        <v>574</v>
+        <v>554</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -17104,10 +17113,10 @@
         <v>373</v>
       </c>
       <c r="B4" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="E4" t="s">
-        <v>573</v>
+        <v>553</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
@@ -17709,41 +17718,41 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>600</v>
+        <v>580</v>
       </c>
       <c r="B2" t="s">
-        <v>587</v>
+        <v>567</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E2" t="s">
-        <v>595</v>
+        <v>575</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>599</v>
+        <v>579</v>
       </c>
       <c r="B3" t="s">
-        <v>588</v>
+        <v>568</v>
       </c>
       <c r="E3" t="s">
-        <v>596</v>
+        <v>576</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>598</v>
+        <v>578</v>
       </c>
       <c r="B4" t="s">
-        <v>589</v>
+        <v>569</v>
       </c>
       <c r="E4" t="s">
-        <v>597</v>
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -17763,7 +17772,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.9" x14ac:dyDescent="0.35"/>
@@ -17895,7 +17904,7 @@
         <v>259</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>583</v>
+        <v>563</v>
       </c>
       <c r="D6" s="71" t="s">
         <v>366</v>
@@ -18042,11 +18051,11 @@
     </row>
     <row r="13" spans="1:12" ht="40.5" x14ac:dyDescent="0.4">
       <c r="A13" s="35" t="s">
-        <v>579</v>
+        <v>559</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="20" t="s">
-        <v>583</v>
+        <v>563</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
@@ -18088,7 +18097,7 @@
         <v>276</v>
       </c>
       <c r="L14" s="61" t="s">
-        <v>586</v>
+        <v>566</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
@@ -18121,7 +18130,7 @@
     <row r="16" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="25"/>
       <c r="B16" s="5" t="s">
-        <v>582</v>
+        <v>562</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>368</v>
@@ -18148,7 +18157,7 @@
     <row r="17" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>368</v>
@@ -18175,7 +18184,7 @@
     <row r="18" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="25"/>
       <c r="B18" s="5" t="s">
-        <v>581</v>
+        <v>561</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>368</v>
@@ -18275,7 +18284,7 @@
       <c r="I21" s="61"/>
       <c r="K21" s="61"/>
       <c r="L21" s="12" t="s">
-        <v>584</v>
+        <v>564</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
@@ -18302,7 +18311,7 @@
       <c r="I22" s="61"/>
       <c r="K22" s="61"/>
       <c r="L22" s="12" t="s">
-        <v>584</v>
+        <v>564</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="13" customFormat="1" ht="27" x14ac:dyDescent="0.35">
@@ -18329,7 +18338,7 @@
       <c r="I23" s="61"/>
       <c r="K23" s="61"/>
       <c r="L23" s="12" t="s">
-        <v>585</v>
+        <v>565</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
@@ -18360,7 +18369,7 @@
     </row>
     <row r="26" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="35" t="s">
-        <v>602</v>
+        <v>582</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -18406,10 +18415,10 @@
     <row r="28" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14"/>
       <c r="B28" s="5" t="s">
-        <v>607</v>
+        <v>587</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -18424,13 +18433,13 @@
       <c r="A29" s="14"/>
       <c r="B29" s="5"/>
       <c r="C29" s="2" t="s">
-        <v>605</v>
+        <v>585</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="31" t="s">
-        <v>605</v>
+        <v>585</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="61"/>
@@ -18476,12 +18485,12 @@
       <c r="K32" s="61"/>
       <c r="L32" s="17"/>
     </row>
-    <row r="33" spans="1:12" s="13" customFormat="1" ht="27.75" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="66" t="s">
-        <v>603</v>
+        <v>583</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="5"/>
@@ -18508,10 +18517,10 @@
     </row>
     <row r="35" spans="1:12" s="13" customFormat="1" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A35" s="35" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>609</v>
+        <v>589</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -29321,8 +29330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29C0825-2196-4293-B771-2CE07AA5FF1C}">
   <dimension ref="A1:L835"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.9" x14ac:dyDescent="0.35"/>
@@ -29342,7 +29351,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="49.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -29397,13 +29406,13 @@
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
       <c r="I3" s="92" t="s">
-        <v>610</v>
+        <v>590</v>
       </c>
       <c r="J3" s="65" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>455</v>
+        <v>655</v>
       </c>
       <c r="L3" s="19"/>
     </row>
@@ -29427,13 +29436,13 @@
         <v>27</v>
       </c>
       <c r="I4" s="93" t="s">
-        <v>611</v>
+        <v>591</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="L4" s="17"/>
     </row>
@@ -29459,23 +29468,23 @@
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="93" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="23" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>657</v>
+        <v>635</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="81" x14ac:dyDescent="0.35">
       <c r="A6" s="22"/>
       <c r="B6" s="94" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
       <c r="C6" s="95" t="s">
-        <v>658</v>
+        <v>636</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
@@ -29491,11 +29500,11 @@
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="93" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="23" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="L6" s="24"/>
     </row>
@@ -29519,11 +29528,11 @@
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="93" t="s">
-        <v>615</v>
+        <v>595</v>
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="23" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="L7" s="33"/>
     </row>
@@ -29547,7 +29556,7 @@
       </c>
       <c r="H8" s="31"/>
       <c r="I8" s="93" t="s">
-        <v>616</v>
+        <v>596</v>
       </c>
       <c r="J8" s="23"/>
       <c r="K8" s="23" t="s">
@@ -29577,21 +29586,21 @@
       </c>
       <c r="H9" s="31"/>
       <c r="I9" s="93" t="s">
-        <v>617</v>
+        <v>597</v>
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="23" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="L9" s="61"/>
     </row>
     <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.35">
       <c r="A10" s="31"/>
       <c r="B10" s="5" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="C10" s="93" t="s">
-        <v>662</v>
+        <v>640</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>3</v>
@@ -29603,27 +29612,27 @@
         <v>5</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="H10" s="31"/>
       <c r="I10" s="93" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
       <c r="J10" s="23"/>
       <c r="K10" s="23" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="L10" s="61" t="s">
-        <v>665</v>
+        <v>643</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.35">
       <c r="A11" s="31"/>
       <c r="B11" s="94" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="C11" s="93" t="s">
-        <v>663</v>
+        <v>641</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>131</v>
@@ -29635,27 +29644,27 @@
         <v>5</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="H11" s="31"/>
       <c r="I11" s="93" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="J11" s="23"/>
       <c r="K11" s="23" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="L11" s="61" t="s">
-        <v>665</v>
+        <v>643</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="27" x14ac:dyDescent="0.35">
       <c r="A12" s="31"/>
       <c r="B12" s="94" t="s">
-        <v>618</v>
+        <v>598</v>
       </c>
       <c r="C12" s="93" t="s">
-        <v>664</v>
+        <v>642</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>131</v>
@@ -29667,25 +29676,25 @@
         <v>5</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="H12" s="31"/>
       <c r="I12" s="93" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
       <c r="J12" s="33"/>
       <c r="K12" s="33" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="L12" s="33"/>
     </row>
-    <row r="13" spans="1:12" ht="94.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="121.5" x14ac:dyDescent="0.35">
       <c r="A13" s="31"/>
       <c r="B13" s="5" t="s">
-        <v>624</v>
+        <v>604</v>
       </c>
       <c r="C13" s="93" t="s">
-        <v>625</v>
+        <v>605</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
@@ -29701,23 +29710,23 @@
       </c>
       <c r="H13" s="31"/>
       <c r="I13" s="93" t="s">
-        <v>628</v>
+        <v>608</v>
       </c>
       <c r="J13" s="23"/>
       <c r="K13" s="23" t="s">
-        <v>460</v>
+        <v>656</v>
       </c>
       <c r="L13" s="61" t="s">
-        <v>659</v>
+        <v>637</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A14" s="31"/>
       <c r="B14" s="94" t="s">
-        <v>626</v>
+        <v>606</v>
       </c>
       <c r="C14" s="93" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
@@ -29733,12 +29742,12 @@
       </c>
       <c r="H14" s="31"/>
       <c r="I14" s="93" t="s">
-        <v>629</v>
+        <v>609</v>
       </c>
       <c r="J14" s="23"/>
       <c r="K14" s="23"/>
       <c r="L14" s="61" t="s">
-        <v>659</v>
+        <v>637</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="27" x14ac:dyDescent="0.35">
@@ -29759,15 +29768,15 @@
         <v>5</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="23" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="J15" s="23"/>
       <c r="K15" s="23" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="L15" s="61"/>
     </row>
@@ -29785,15 +29794,15 @@
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H16" s="31"/>
       <c r="I16" s="93" t="s">
-        <v>630</v>
+        <v>610</v>
       </c>
       <c r="J16" s="23"/>
       <c r="K16" s="23" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="L16" s="33"/>
     </row>
@@ -29827,11 +29836,11 @@
     </row>
     <row r="19" spans="1:12" ht="67.5" x14ac:dyDescent="0.4">
       <c r="A19" s="66" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="20" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
@@ -29839,11 +29848,11 @@
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="92" t="s">
-        <v>631</v>
+        <v>611</v>
       </c>
       <c r="J19" s="19"/>
       <c r="K19" s="19" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="L19" s="36"/>
     </row>
@@ -29865,15 +29874,15 @@
         <v>5</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H20" s="23"/>
       <c r="I20" s="17" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="J20" s="17"/>
       <c r="K20" s="17" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="L20" s="76"/>
     </row>
@@ -29895,22 +29904,22 @@
         <v>5</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H21" s="23"/>
       <c r="I21" s="15" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="L21" s="12"/>
     </row>
     <row r="22" spans="1:12" s="13" customFormat="1" ht="81" x14ac:dyDescent="0.35">
       <c r="A22" s="25"/>
       <c r="B22" s="94" t="s">
-        <v>633</v>
+        <v>613</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>136</v>
@@ -29929,23 +29938,23 @@
       </c>
       <c r="H22" s="31"/>
       <c r="I22" s="97" t="s">
-        <v>638</v>
+        <v>618</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="17" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>632</v>
+        <v>612</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="13" customFormat="1" ht="54" x14ac:dyDescent="0.35">
       <c r="A23" s="25"/>
       <c r="B23" s="94" t="s">
-        <v>634</v>
+        <v>614</v>
       </c>
       <c r="C23" s="95" t="s">
-        <v>636</v>
+        <v>616</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
@@ -29961,22 +29970,22 @@
       </c>
       <c r="H23" s="31"/>
       <c r="I23" s="93" t="s">
-        <v>639</v>
+        <v>619</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>474</v>
+        <v>657</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="13" customFormat="1" ht="81" x14ac:dyDescent="0.35">
       <c r="A24" s="25"/>
       <c r="B24" s="94" t="s">
-        <v>635</v>
+        <v>615</v>
       </c>
       <c r="C24" s="96" t="s">
-        <v>637</v>
+        <v>617</v>
       </c>
       <c r="D24" s="32">
         <v>1</v>
@@ -29992,11 +30001,11 @@
       </c>
       <c r="H24" s="31"/>
       <c r="I24" s="93" t="s">
-        <v>640</v>
+        <v>620</v>
       </c>
       <c r="J24" s="17"/>
       <c r="K24" s="17" t="s">
-        <v>480</v>
+        <v>649</v>
       </c>
       <c r="L24" s="33"/>
     </row>
@@ -30056,13 +30065,13 @@
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
     </row>
-    <row r="29" spans="1:12" ht="67.5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" ht="81" x14ac:dyDescent="0.4">
       <c r="A29" s="66" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="20" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
@@ -30070,11 +30079,11 @@
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
       <c r="I29" s="92" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="J29" s="19"/>
       <c r="K29" s="19" t="s">
-        <v>477</v>
+        <v>659</v>
       </c>
       <c r="L29" s="36"/>
     </row>
@@ -30096,15 +30105,15 @@
         <v>5</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H30" s="23"/>
       <c r="I30" s="97" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
       <c r="J30" s="17"/>
       <c r="K30" s="97" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="L30" s="76"/>
     </row>
@@ -30126,25 +30135,25 @@
         <v>5</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H31" s="23"/>
       <c r="I31" s="17" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="17" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12" s="13" customFormat="1" ht="54" x14ac:dyDescent="0.35">
       <c r="A32" s="25"/>
       <c r="B32" s="94" t="s">
-        <v>634</v>
+        <v>614</v>
       </c>
       <c r="C32" s="95" t="s">
-        <v>636</v>
+        <v>616</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
@@ -30160,23 +30169,23 @@
       </c>
       <c r="H32" s="31"/>
       <c r="I32" s="93" t="s">
-        <v>644</v>
+        <v>624</v>
       </c>
       <c r="J32" s="17"/>
       <c r="K32" s="17" t="s">
-        <v>474</v>
+        <v>657</v>
       </c>
       <c r="L32" s="12" t="s">
-        <v>660</v>
+        <v>638</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="13" customFormat="1" ht="81" x14ac:dyDescent="0.35">
       <c r="A33" s="25"/>
       <c r="B33" s="94" t="s">
-        <v>635</v>
+        <v>615</v>
       </c>
       <c r="C33" s="93" t="s">
-        <v>637</v>
+        <v>617</v>
       </c>
       <c r="D33" s="32">
         <v>1</v>
@@ -30192,23 +30201,23 @@
       </c>
       <c r="H33" s="31"/>
       <c r="I33" s="93" t="s">
-        <v>645</v>
+        <v>625</v>
       </c>
       <c r="J33" s="17"/>
       <c r="K33" s="17" t="s">
-        <v>480</v>
+        <v>658</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>660</v>
+        <v>638</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="13" customFormat="1" ht="108" x14ac:dyDescent="0.35">
       <c r="A34" s="25"/>
       <c r="B34" s="5" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="D34" s="5">
         <v>1</v>
@@ -30224,14 +30233,14 @@
       </c>
       <c r="H34" s="31"/>
       <c r="I34" s="97" t="s">
-        <v>666</v>
+        <v>644</v>
       </c>
       <c r="J34" s="17"/>
       <c r="K34" s="17" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="L34" s="12" t="s">
-        <v>643</v>
+        <v>623</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
@@ -30278,11 +30287,11 @@
     </row>
     <row r="38" spans="1:12" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A38" s="66" t="s">
-        <v>505</v>
+        <v>661</v>
       </c>
       <c r="B38" s="19"/>
       <c r="C38" s="20" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
@@ -30290,13 +30299,15 @@
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
       <c r="I38" s="19" t="s">
-        <v>484</v>
+        <v>645</v>
       </c>
       <c r="J38" s="19"/>
       <c r="K38" s="19" t="s">
-        <v>506</v>
-      </c>
-      <c r="L38" s="77"/>
+        <v>651</v>
+      </c>
+      <c r="L38" s="77" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="39" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="25"/>
@@ -30316,25 +30327,25 @@
         <v>5</v>
       </c>
       <c r="G39" s="23" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H39" s="23"/>
       <c r="I39" s="17" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="J39" s="17"/>
       <c r="K39" s="17" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="L39" s="17"/>
     </row>
     <row r="40" spans="1:12" s="13" customFormat="1" ht="27" x14ac:dyDescent="0.35">
       <c r="A40" s="25"/>
       <c r="B40" s="5" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>487</v>
+        <v>646</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>3</v>
@@ -30346,15 +30357,15 @@
         <v>5</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="17" t="s">
-        <v>486</v>
+        <v>662</v>
       </c>
       <c r="J40" s="17"/>
       <c r="K40" s="17" t="s">
-        <v>485</v>
+        <v>652</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.35">
@@ -30398,13 +30409,13 @@
       <c r="K43" s="29"/>
       <c r="L43" s="29"/>
     </row>
-    <row r="44" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.35">
       <c r="A44" s="66" t="s">
-        <v>488</v>
+        <v>666</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="2" t="s">
-        <v>487</v>
+        <v>646</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -30414,14 +30425,16 @@
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-    </row>
-    <row r="45" spans="1:12" s="4" customFormat="1" ht="108" x14ac:dyDescent="0.35">
+      <c r="L44" s="61" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="4" customFormat="1" ht="121.5" x14ac:dyDescent="0.35">
       <c r="B45" s="5" t="s">
-        <v>646</v>
+        <v>626</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>647</v>
+        <v>627</v>
       </c>
       <c r="D45" s="94">
         <v>1</v>
@@ -30433,26 +30446,24 @@
         <v>5</v>
       </c>
       <c r="G45" s="23" t="s">
-        <v>404</v>
+        <v>668</v>
       </c>
       <c r="H45" s="23"/>
       <c r="I45" s="17" t="s">
-        <v>648</v>
+        <v>663</v>
       </c>
       <c r="J45" s="17"/>
       <c r="K45" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>649</v>
-      </c>
+        <v>650</v>
+      </c>
+      <c r="L45" s="12"/>
     </row>
     <row r="46" spans="1:12" s="4" customFormat="1" ht="67.5" x14ac:dyDescent="0.35">
       <c r="B46" s="5" t="s">
-        <v>406</v>
+        <v>664</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>405</v>
+        <v>647</v>
       </c>
       <c r="D46" s="5">
         <v>1</v>
@@ -30468,21 +30479,21 @@
       </c>
       <c r="H46" s="23"/>
       <c r="I46" s="17" t="s">
-        <v>490</v>
+        <v>665</v>
       </c>
       <c r="J46" s="17"/>
       <c r="K46" s="17" t="s">
-        <v>489</v>
+        <v>653</v>
       </c>
       <c r="L46" s="17"/>
     </row>
-    <row r="47" spans="1:12" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" s="4" customFormat="1" ht="121.5" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="5" t="s">
         <v>181</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>491</v>
+        <v>648</v>
       </c>
       <c r="D47" s="94" t="s">
         <v>2</v>
@@ -30494,15 +30505,15 @@
         <v>5</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>491</v>
+        <v>648</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="17" t="s">
-        <v>495</v>
+        <v>667</v>
       </c>
       <c r="J47" s="15"/>
       <c r="K47" s="33" t="s">
-        <v>494</v>
+        <v>654</v>
       </c>
       <c r="L47" s="15"/>
     </row>
@@ -30550,11 +30561,11 @@
     </row>
     <row r="51" spans="1:12" s="4" customFormat="1" ht="54" x14ac:dyDescent="0.35">
       <c r="A51" s="42" t="s">
-        <v>507</v>
+        <v>487</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="2" t="s">
-        <v>491</v>
+        <v>648</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -30562,11 +30573,11 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="33" t="s">
-        <v>492</v>
+        <v>477</v>
       </c>
       <c r="J51" s="15"/>
       <c r="K51" s="23" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
       <c r="L51" s="15"/>
     </row>
@@ -30591,11 +30602,11 @@
         <v>86</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="J52" s="15"/>
       <c r="K52" s="15" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="L52" s="15"/>
     </row>
@@ -30620,23 +30631,23 @@
         <v>300</v>
       </c>
       <c r="I53" s="95" t="s">
-        <v>650</v>
+        <v>628</v>
       </c>
       <c r="J53" s="15"/>
-      <c r="K53" s="15" t="s">
-        <v>497</v>
+      <c r="K53" s="33" t="s">
+        <v>479</v>
       </c>
       <c r="L53" s="61" t="s">
-        <v>651</v>
+        <v>629</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="4" customFormat="1" ht="54" x14ac:dyDescent="0.35">
       <c r="A54" s="13"/>
       <c r="B54" s="4" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D54" s="4">
         <v>1</v>
@@ -30651,20 +30662,20 @@
         <v>15</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="55" spans="1:12" s="4" customFormat="1" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D55" s="4">
         <v>1</v>
@@ -30679,11 +30690,11 @@
         <v>15</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="J55" s="33"/>
       <c r="K55" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="L55" s="15"/>
     </row>
@@ -30728,11 +30739,11 @@
       <c r="G58" s="20"/>
       <c r="H58" s="20"/>
       <c r="I58" s="92" t="s">
-        <v>652</v>
+        <v>630</v>
       </c>
       <c r="J58" s="19"/>
       <c r="K58" s="19" t="s">
-        <v>526</v>
+        <v>506</v>
       </c>
       <c r="L58" s="77"/>
     </row>
@@ -30753,10 +30764,10 @@
         <v>86</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I59" s="94" t="s">
-        <v>653</v>
+        <v>631</v>
       </c>
       <c r="K59" s="5" t="s">
         <v>297</v>
@@ -30784,13 +30795,13 @@
         <v>300</v>
       </c>
       <c r="H60" s="17" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I60" s="97" t="s">
-        <v>654</v>
+        <v>632</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="L60" s="15"/>
     </row>
@@ -30817,7 +30828,7 @@
         <v>350</v>
       </c>
       <c r="I61" s="94" t="s">
-        <v>655</v>
+        <v>633</v>
       </c>
       <c r="K61" s="5" t="s">
         <v>303</v>
@@ -30848,7 +30859,7 @@
         <v>351</v>
       </c>
       <c r="I62" s="94" t="s">
-        <v>656</v>
+        <v>634</v>
       </c>
       <c r="K62" s="5" t="s">
         <v>304</v>
@@ -41687,7 +41698,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -41722,10 +41733,10 @@
         <v>187</v>
       </c>
       <c r="G1" s="79" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H1" s="79" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -41736,10 +41747,10 @@
         <v>234</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E2" t="s">
         <v>237</v>
@@ -41753,13 +41764,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="80" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B3" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -41770,13 +41781,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B4" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E4" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -41787,13 +41798,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B5" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E5" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -41804,13 +41815,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E6" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -41821,13 +41832,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B7" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E7" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -41838,13 +41849,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B8" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E8" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -41891,13 +41902,13 @@
         <v>287</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>514</v>
+        <v>494</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>515</v>
+        <v>495</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>187</v>
@@ -41924,7 +41935,7 @@
     </row>
     <row r="2" spans="1:13" ht="27" x14ac:dyDescent="0.35">
       <c r="A2" s="81" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B2" s="73" t="s">
         <v>36</v>
@@ -42834,13 +42845,13 @@
         <v>287</v>
       </c>
       <c r="C1" s="82" t="s">
-        <v>518</v>
+        <v>498</v>
       </c>
       <c r="D1" s="82" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="E1" s="82" t="s">
-        <v>517</v>
+        <v>497</v>
       </c>
       <c r="F1" s="82" t="s">
         <v>187</v>
@@ -42852,15 +42863,15 @@
         <v>292</v>
       </c>
       <c r="I1" s="82" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="J1" s="82" t="s">
-        <v>537</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A2" s="84" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -42895,13 +42906,13 @@
         <v>287</v>
       </c>
       <c r="C1" s="82" t="s">
-        <v>518</v>
+        <v>498</v>
       </c>
       <c r="D1" s="82" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="E1" s="82" t="s">
-        <v>517</v>
+        <v>497</v>
       </c>
       <c r="F1" s="82" t="s">
         <v>187</v>
@@ -42909,7 +42920,7 @@
     </row>
     <row r="2" spans="1:6" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A2" s="84" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -43107,15 +43118,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="25bcd8d1-946a-40fe-b23d-435fd4bd57a8" xsi:nil="true"/>
@@ -43125,6 +43127,15 @@
     </f55088e9522d40e68e870fa734a74ee1>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -43147,14 +43158,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71BD380-CB64-4C21-84F9-8F5250655069}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EDA3539-A5DD-4DC3-8F1D-F5FC9E86B407}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -43169,4 +43172,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71BD380-CB64-4C21-84F9-8F5250655069}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>